<commit_message>
mapping raw data file to get multiple sheets
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\xlsx-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DB71EA-0558-46B5-BD77-D50112E427DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B667DE-81C9-4A64-A5C4-AA904A14D4CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B6BBAC30-48E3-DE4C-89C4-AC71FE5D2887}"/>
   </bookViews>
@@ -22,9 +22,9 @@
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="5" r:id="rId8"/>
-    <pivotCache cacheId="9" r:id="rId9"/>
+    <pivotCache cacheId="58" r:id="rId7"/>
+    <pivotCache cacheId="64" r:id="rId8"/>
+    <pivotCache cacheId="67" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="57">
   <si>
     <t>CÔNG TY CỔ PHẦN HỆ THỐNG THÔNG TIN FPT</t>
   </si>
@@ -142,12 +142,6 @@
     <t>4000$</t>
   </si>
   <si>
-    <t>${table:rawData.C}</t>
-  </si>
-  <si>
-    <t>${table:rawData.D}</t>
-  </si>
-  <si>
     <t>Row Labels</t>
   </si>
   <si>
@@ -163,24 +157,6 @@
     <t>Chi phí</t>
   </si>
   <si>
-    <t>${table:rawData2.A}</t>
-  </si>
-  <si>
-    <t>${table:rawData2.B}</t>
-  </si>
-  <si>
-    <t>${table:rawData3.A}</t>
-  </si>
-  <si>
-    <t>${table:rawData3.B}</t>
-  </si>
-  <si>
-    <t>${table:rawData3.C}</t>
-  </si>
-  <si>
-    <t>${table:rawData3.D}</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -202,10 +178,34 @@
     <t>Count of Giá trị</t>
   </si>
   <si>
-    <t>${table:A.A}</t>
-  </si>
-  <si>
-    <t>${table:B.B}</t>
+    <t>${C}</t>
+  </si>
+  <si>
+    <t>${D}</t>
+  </si>
+  <si>
+    <t>${table:2.A}</t>
+  </si>
+  <si>
+    <t>${table:2.B}</t>
+  </si>
+  <si>
+    <t>${table:23.A}</t>
+  </si>
+  <si>
+    <t>${table:23.B}</t>
+  </si>
+  <si>
+    <t>${table:23.C}</t>
+  </si>
+  <si>
+    <t>${table:23.D}</t>
+  </si>
+  <si>
+    <t>${table:2.C}</t>
+  </si>
+  <si>
+    <t>${table:2.D}</t>
   </si>
 </sst>
 </file>
@@ -311,11 +311,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -796,7 +796,7 @@
   </mc:AlternateContent>
   <c:pivotSource>
     <c:name>[template.xlsx]Template!PivotTable6</c:name>
-    <c:fmtId val="1"/>
+    <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
@@ -938,7 +938,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-0AA9-488F-AA1B-B9F2139318BB}"/>
+                <c16:uniqueId val="{00000001-381C-46DD-99E9-F3644EE2A194}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -967,7 +967,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D2A6-4406-96F4-EC74E8AD51F0}"/>
+              <c16:uniqueId val="{00000000-639A-476B-B8A5-C524E6E451A0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1618,12 +1618,12 @@
                 <c:ptCount val="1"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>${table:rawData.D}</c:v>
+                    <c:v>${table:2.D}</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>${table:B.B}</c:v>
+                    <c:v>${table:2.B}</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -3557,22 +3557,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2905125</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="21" name="Chart 20">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2E40E27-BDBA-44A5-A22F-00A7DEC31432}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABBC8A11-5C64-4FB4-93F9-8911F2A94CB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3671,7 +3671,41 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="ADMIN" refreshedDate="44321.72921539352" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="1" xr:uid="{C18BAD27-3803-4F54-963B-37140FF4603A}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="ADMIN" refreshedDate="44322.585702893521" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="1" xr:uid="{FD5FC87F-6850-4CDE-93F3-23284B3414DB}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1349"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Nội dung công việc" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Người phụ trách" numFmtId="0">
+      <sharedItems count="3">
+        <s v="${table:2.B}"/>
+        <s v="${table:B.B}" u="1"/>
+        <s v="${table:rawData.B}" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Mức độ ưu tiên" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Tình trạng" numFmtId="0">
+      <sharedItems count="2">
+        <s v="${table:2.D}"/>
+        <s v="${table:rawData.D}" u="1"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="ADMIN" refreshedDate="44322.585703240744" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="1" xr:uid="{C18BAD27-3803-4F54-963B-37140FF4603A}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -3683,38 +3717,6 @@
     </cacheField>
     <cacheField name="Giá trị" numFmtId="0">
       <sharedItems/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="ADMIN" refreshedDate="44321.729215509258" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="1" xr:uid="{FD5FC87F-6850-4CDE-93F3-23284B3414DB}">
-  <cacheSource type="worksheet">
-    <worksheetSource name="Table1349"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Nội dung công việc" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Người phụ trách" numFmtId="0">
-      <sharedItems count="2">
-        <s v="${table:B.B}"/>
-        <s v="${table:rawData.B}" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Mức độ ưu tiên" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Tình trạng" numFmtId="0">
-      <sharedItems count="1">
-        <s v="${table:rawData.D}"/>
-      </sharedItems>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -3775,8 +3777,10 @@
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
+    <s v="${table:2.A}"/>
     <x v="0"/>
-    <s v="${table:newData.G}"/>
+    <s v="${table:2.C}"/>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -3784,16 +3788,14 @@
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
-    <s v="${table:A.A}"/>
     <x v="0"/>
-    <s v="${table:rawData.C}"/>
-    <x v="0"/>
+    <s v="${table:newData.G}"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{17FD627B-B9D8-3048-9F14-21F743907651}" name="PivotTable10" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{17FD627B-B9D8-3048-9F14-21F743907651}" name="PivotTable10" cacheId="58" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="H13:I24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
@@ -3885,7 +3887,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BBE8DDBE-E0FC-4136-9C6C-7809931EE6D5}" name="PivotTable6" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BBE8DDBE-E0FC-4136-9C6C-7809931EE6D5}" name="PivotTable6" cacheId="67" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="F28:G30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -3913,7 +3915,7 @@
   <dataFields count="1">
     <dataField name="Count of Giá trị" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="4">
     <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3924,6 +3926,27 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="1" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -3949,12 +3972,13 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7496FED7-E595-41CB-B0D1-56BA4B2F9F5F}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7496FED7-E595-41CB-B0D1-56BA4B2F9F5F}" name="PivotTable1" cacheId="64" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="3">
+      <items count="4">
+        <item m="1" x="2"/>
         <item m="1" x="1"/>
         <item x="0"/>
         <item t="default"/>
@@ -3962,7 +3986,8 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="2">
+      <items count="3">
+        <item m="1" x="1"/>
         <item x="0"/>
         <item t="default"/>
       </items>
@@ -3974,10 +3999,10 @@
   </rowFields>
   <rowItems count="3">
     <i>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
-      <x/>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -4484,10 +4509,10 @@
         <v>10</v>
       </c>
       <c r="H13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
         <v>37</v>
-      </c>
-      <c r="I13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -4654,7 +4679,7 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>14</v>
@@ -4671,7 +4696,7 @@
         <v>0.15</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I24" s="9">
         <v>7</v>
@@ -4703,7 +4728,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4745,7 +4770,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4765,10 +4790,16 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -4813,7 +4844,7 @@
       </c>
       <c r="B7" s="18"/>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -4822,7 +4853,7 @@
       </c>
       <c r="B8" s="18"/>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -4831,7 +4862,7 @@
       </c>
       <c r="B9" s="18"/>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4840,7 +4871,7 @@
       </c>
       <c r="B10" s="18"/>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -4868,27 +4899,27 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
         <v>55</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -4901,36 +4932,36 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F28" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F29" s="14" t="s">
-        <v>52</v>
+      <c r="F29" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="G29" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F30" s="14" t="s">
-        <v>38</v>
+      <c r="F30" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="G30" s="9">
         <v>1</v>
@@ -4986,8 +5017,8 @@
       <c r="G1" s="11">
         <v>0.15</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="15"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
@@ -5135,16 +5166,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -5157,12 +5188,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="25.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
@@ -5170,15 +5201,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>56</v>
+      <c r="A2" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -5186,15 +5217,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>38</v>
+      <c r="A4" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>

</xml_diff>